<commit_message>
feat: update cras streamlit
</commit_message>
<xml_diff>
--- a/feature_display_info.xlsx
+++ b/feature_display_info.xlsx
@@ -1786,7 +1786,7 @@
   <sheetPr/>
   <dimension ref="A1:I16384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
@@ -3243,7 +3243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" ht="14.25" spans="1:6">
       <c r="A97" s="2" t="s">
         <v>189</v>
       </c>

</xml_diff>